<commit_message>
Ferammenta integrada com o mongo atlas
</commit_message>
<xml_diff>
--- a/backEnd/webScraping/Backup/socialFinance.xlsx
+++ b/backEnd/webScraping/Backup/socialFinance.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A139"/>
+  <dimension ref="A1:A277"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1406,6 +1406,972 @@
         </is>
       </c>
     </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>project_index_136</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>project_index_135</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>project_index_137</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>project_index_130</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>project_index_129</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>project_index_127</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>project_index_124</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>project_index_123</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>project_index_116</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>project_index_126</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>project_index_128</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>project_index_134</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>project_index_133</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>project_index_125</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>project_index_113</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>project_index_112</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>project_index_119</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>project_index_115</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>project_index_3</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>project_index_121</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>project_index_120</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>project_index_122</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>project_index_132</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>project_index_109</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>project_index_108</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>project_index_74</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>project_index_107</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>project_index_105</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>project_index_104</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>project_index_103</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>project_index_106</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>project_index_101</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>project_index_5</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>project_index_110</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>project_index_6</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>project_index_102</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>project_index_117</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>project_index_111</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>project_index_99</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>project_index_98</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>project_index_97</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>project_index_100</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>project_index_131</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>project_index_96</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>project_index_86</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>project_index_10</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>project_index_0</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>project_index_89</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>project_index_88</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>project_index_90</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>project_index_114</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>project_index_95</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>project_index_11</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>project_index_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>project_index_1</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>project_index_85</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>project_index_94</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>project_index_92</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>project_index_91</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>project_index_118</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>project_index_84</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>project_index_77</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>project_index_70</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>project_index_82</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>project_index_81</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>project_index_80</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>project_index_79</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>project_index_83</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>project_index_76</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>project_index_73</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>project_index_72</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>project_index_68</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>project_index_78</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>project_index_93</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>project_index_75</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>project_index_69</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>project_index_67</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>project_index_71</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>project_index_87</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>project_index_66</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>project_index_65</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>project_index_64</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>project_index_63</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>project_index_62</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>project_index_61</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>project_index_60</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>project_index_59</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>project_index_57</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>project_index_4</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>project_index_58</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>project_index_56</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>project_index_55</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>project_index_54</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>project_index_53</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>project_index_51</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>project_index_49</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>project_index_48</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>project_index_50</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>project_index_46</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>project_index_52</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>project_index_47</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>project_index_44</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>project_index_42</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>project_index_41</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>project_index_40</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>project_index_39</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>project_index_38</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>project_index_45</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>project_index_43</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>project_index_37</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>project_index_36</t>
+        </is>
+      </c>
+    </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>project_index_35</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>project_index_34</t>
+        </is>
+      </c>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>project_index_33</t>
+        </is>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>project_index_32</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>project_index_31</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>project_index_29</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>project_index_30</t>
+        </is>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>project_index_28</t>
+        </is>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>project_index_26</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>project_index_27</t>
+        </is>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>project_index_25</t>
+        </is>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>project_index_24</t>
+        </is>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>project_index_16</t>
+        </is>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>project_index_20</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>project_index_17</t>
+        </is>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>project_index_19</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>project_index_18</t>
+        </is>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>project_index_22</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>project_index_21</t>
+        </is>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>project_index_23</t>
+        </is>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>project_index_15</t>
+        </is>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>project_index_9</t>
+        </is>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>project_index_13</t>
+        </is>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>project_index_14</t>
+        </is>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>project_index_12</t>
+        </is>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>project_index_8</t>
+        </is>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>project_index_7</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>